<commit_message>
finished integrating literature update for now
</commit_message>
<xml_diff>
--- a/Midterm Report/Selection of Prompt Engineering Methods/hand-labeled method and implementation considerations.xlsx
+++ b/Midterm Report/Selection of Prompt Engineering Methods/hand-labeled method and implementation considerations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\anlp23-project\Midterm Report\Selection of Prompt Engineering Methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865F3607-9A65-4AC8-9F6D-9A5DA84534AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712310D5-D826-4D26-96FD-DD8F7A0DEA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="140">
   <si>
     <t>Title</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>Performance Gain</t>
+  </si>
+  <si>
+    <t>Datasets</t>
   </si>
 </sst>
 </file>
@@ -508,10 +511,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -822,15 +825,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.33203125" customWidth="1"/>
+    <col min="1" max="1" width="94" customWidth="1"/>
     <col min="2" max="2" width="43.5546875" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="4" max="4" width="13.21875" style="4" bestFit="1" customWidth="1"/>
@@ -839,7 +842,7 @@
     <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -861,8 +864,11 @@
       <c r="G1" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -882,7 +888,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -899,7 +905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -916,7 +922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -933,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -950,7 +956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -970,7 +976,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -981,7 +987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -992,7 +998,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1003,7 +1009,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1022,7 +1028,7 @@
         <v>0.65593220338983049</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1030,7 +1036,7 @@
         <v>0.63755458515283847</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1038,7 +1044,7 @@
         <v>0.59105098855359006</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1046,7 +1052,7 @@
         <v>0.53086419753086422</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
major rework of popularity project
</commit_message>
<xml_diff>
--- a/Midterm Report/Selection of Prompt Engineering Methods/hand-labeled method and implementation considerations.xlsx
+++ b/Midterm Report/Selection of Prompt Engineering Methods/hand-labeled method and implementation considerations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\anlp23-project\Midterm Report\Selection of Prompt Engineering Methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712310D5-D826-4D26-96FD-DD8F7A0DEA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A97E85A-2E41-4523-BB9B-F189FD8247DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -828,16 +828,16 @@
   <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="94" customWidth="1"/>
     <col min="2" max="2" width="43.5546875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="37" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.88671875" style="4" customWidth="1"/>
     <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
start of day 10-23-23 save
</commit_message>
<xml_diff>
--- a/Midterm Report/Selection of Prompt Engineering Methods/hand-labeled method and implementation considerations.xlsx
+++ b/Midterm Report/Selection of Prompt Engineering Methods/hand-labeled method and implementation considerations.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\anlp23-project\Midterm Report\Selection of Prompt Engineering Methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C84C157-9821-4028-AECB-548BAD7B9E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EA03EE-2E6B-4DDC-A420-595989EEC872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="381">
   <si>
     <t>paper title</t>
   </si>
@@ -1019,6 +1032,150 @@
   </si>
   <si>
     <t>AI Safety</t>
+  </si>
+  <si>
+    <t>GSM8K, PIE, CommonGen, CodeNet</t>
+  </si>
+  <si>
+    <t>For each type of task, write a feedback prompt/rubric the model can score itself on</t>
+  </si>
+  <si>
+    <t>HotpotQA, Fever, ALFWorld, WebShop</t>
+  </si>
+  <si>
+    <t>Would require hookup to external knowledge bases. Similar to web browsing for GPT-X, but not really implementable for older models</t>
+  </si>
+  <si>
+    <t>10-34%</t>
+  </si>
+  <si>
+    <t>Requires vector knowledge sources</t>
+  </si>
+  <si>
+    <t>Natural Questions, WebQuestions, CuratedTrec, TriviaQA, MS-MARCO, Fever</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Retrieval-Augmented-Generation</t>
+  </si>
+  <si>
+    <t>Good paper concerning the importance of the label space, distribution of input text, etc. for few-shot prompting</t>
+  </si>
+  <si>
+    <t>Last Letter, SCAN, GSM8K, DROP</t>
+  </si>
+  <si>
+    <t>See page 58 examples. "Let's break down this problem." Usage of engineered examples can lead to improvement. Overall this is a tricky variant of chain-of-thought prompting. But overall examples can be repeated</t>
+  </si>
+  <si>
+    <t>0-15%</t>
+  </si>
+  <si>
+    <t>Considered earlier as a list of approaches but not chosen</t>
+  </si>
+  <si>
+    <t>New multimodal language model</t>
+  </si>
+  <si>
+    <t>Contextual Calibration</t>
+  </si>
+  <si>
+    <t>SST-2, TREC, CB, RTE, AGNews, DBPedia, LAMA, ATIS, MIT Movies</t>
+  </si>
+  <si>
+    <t>Varying example order, prompt format, majority label, recency, common token bias. Requires output probabilities for bias correction</t>
+  </si>
+  <si>
+    <t>Program Aided Language Models</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Hooking up models to Python interpreter, etc. Unclear if its worth exploring given ubiquity of Code Interpreter. Also not super generalizable to reasoning tasks</t>
+  </si>
+  <si>
+    <t>Big-Bench Instruction Induction (BBII), Big-Bench Hard</t>
+  </si>
+  <si>
+    <t>Surpassing human-level prompt engineering in some cases. Iterative Monte-Carlo search. Source of "Let's work this out in a step by step way to be sure…"</t>
+  </si>
+  <si>
+    <t>LAMA</t>
+  </si>
+  <si>
+    <t>Fill in the blank tasks only</t>
+  </si>
+  <si>
+    <t>Prompt Mining, Prompt Paraphrasing</t>
+  </si>
+  <si>
+    <t>Interestingly does consider costs of the method as they are high</t>
+  </si>
+  <si>
+    <t>Graph of Thoughts</t>
+  </si>
+  <si>
+    <t>Custom - Sorting, Set Operations, Keyword Counting, Document Merging</t>
+  </si>
+  <si>
+    <t>Automatic Chain of Thought Prompting</t>
+  </si>
+  <si>
+    <t>MultiArith, GSM8K, CommonSenseQA, SVAMP, AQUA-RAT, StrategyQA, Last Letter, Coin Flip</t>
+  </si>
+  <si>
+    <t>5-10%</t>
+  </si>
+  <si>
+    <t>Sample questions and generate reasoning chains to construct demonstrations. Requires usage of BERT embeddings for question clustering, sampling from clusters, and then using zero-shot CoT on questions to create final demonstrations</t>
+  </si>
+  <si>
+    <t>Long addition, division, execution of arbitrary programs</t>
+  </si>
+  <si>
+    <t>Scratchpads</t>
+  </si>
+  <si>
+    <t>10-15%</t>
+  </si>
+  <si>
+    <t>Could maybe do scratchpads for non-math/code tasks. This would potentially be trickier to do via prompting as opposed to using underly algorithms like in the paper</t>
+  </si>
+  <si>
+    <t>Few-shot Retrieval Augmented Generation</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>NaturalQuestions, TriviaQA, FEVER, MMLU, KILT</t>
+  </si>
+  <si>
+    <t>3-10%</t>
+  </si>
+  <si>
+    <t>Requires retriever architecture</t>
+  </si>
+  <si>
+    <t>Requires sampling of the language model itself</t>
+  </si>
+  <si>
+    <t>SST, DBPedia, MR, CR, MPQA, Subj, TREC, AGNews, RTE, CB</t>
+  </si>
+  <si>
+    <t>Few-shot Prompt Ordering</t>
+  </si>
+  <si>
+    <t>MathMix, MATH</t>
+  </si>
+  <si>
+    <t>Process rather than outcome supervision. Uses outcome and reward models, unfortunately</t>
+  </si>
+  <si>
+    <t>Process Supervision</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1085,11 +1242,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1109,6 +1275,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1411,10 +1580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P162"/>
+  <dimension ref="A1:S162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="K27" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,7 +1599,7 @@
     <col min="10" max="10" width="16.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1480,7 +1649,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1530,7 +1699,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1579,8 +1748,9 @@
       <c r="P3" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1630,7 +1800,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1680,7 +1850,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1730,7 +1900,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1780,7 +1950,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1830,7 +2000,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1880,7 +2050,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1930,7 +2100,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1980,7 +2150,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2030,7 +2200,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -2080,7 +2250,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -2130,7 +2300,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2180,7 +2350,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2214,8 +2384,23 @@
       <c r="K16" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" t="s">
+        <v>287</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="O16" t="s">
+        <v>334</v>
+      </c>
+      <c r="P16" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2249,8 +2434,23 @@
       <c r="K17" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17" t="s">
+        <v>287</v>
+      </c>
+      <c r="M17">
+        <v>4</v>
+      </c>
+      <c r="N17" t="s">
+        <v>337</v>
+      </c>
+      <c r="O17" t="s">
+        <v>336</v>
+      </c>
+      <c r="P17" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2281,8 +2481,26 @@
       <c r="J18">
         <v>0.76567923536422988</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K18" t="s">
+        <v>341</v>
+      </c>
+      <c r="L18" t="s">
+        <v>371</v>
+      </c>
+      <c r="M18">
+        <v>5</v>
+      </c>
+      <c r="N18" t="s">
+        <v>340</v>
+      </c>
+      <c r="O18" t="s">
+        <v>338</v>
+      </c>
+      <c r="P18" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -2313,8 +2531,26 @@
       <c r="J19">
         <v>0.71290973543928726</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K19" t="s">
+        <v>307</v>
+      </c>
+      <c r="L19" t="s">
+        <v>307</v>
+      </c>
+      <c r="M19" t="s">
+        <v>307</v>
+      </c>
+      <c r="N19" t="s">
+        <v>307</v>
+      </c>
+      <c r="O19" t="s">
+        <v>342</v>
+      </c>
+      <c r="P19" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -2348,8 +2584,23 @@
       <c r="K20" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" t="s">
+        <v>287</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20" t="s">
+        <v>345</v>
+      </c>
+      <c r="O20" t="s">
+        <v>344</v>
+      </c>
+      <c r="P20" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2380,8 +2631,26 @@
       <c r="J21">
         <v>0.66922693081589502</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
+        <v>307</v>
+      </c>
+      <c r="L21" t="s">
+        <v>307</v>
+      </c>
+      <c r="M21" t="s">
+        <v>307</v>
+      </c>
+      <c r="N21" t="s">
+        <v>307</v>
+      </c>
+      <c r="O21" t="s">
+        <v>346</v>
+      </c>
+      <c r="P21" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -2412,8 +2681,26 @@
       <c r="J22">
         <v>0.64824468812237357</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K22" t="s">
+        <v>307</v>
+      </c>
+      <c r="L22" t="s">
+        <v>307</v>
+      </c>
+      <c r="M22" t="s">
+        <v>307</v>
+      </c>
+      <c r="N22" t="s">
+        <v>307</v>
+      </c>
+      <c r="O22" t="s">
+        <v>347</v>
+      </c>
+      <c r="P22" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2444,8 +2731,26 @@
       <c r="J23">
         <v>0.63142921575299549</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K23" t="s">
+        <v>348</v>
+      </c>
+      <c r="L23" t="s">
+        <v>287</v>
+      </c>
+      <c r="M23">
+        <v>5</v>
+      </c>
+      <c r="N23" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="O23" t="s">
+        <v>350</v>
+      </c>
+      <c r="P23" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2476,8 +2781,23 @@
       <c r="J24">
         <v>0.58482189517385985</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K24" t="s">
+        <v>351</v>
+      </c>
+      <c r="L24" t="s">
+        <v>352</v>
+      </c>
+      <c r="M24">
+        <v>4</v>
+      </c>
+      <c r="N24" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="O24" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2511,8 +2831,23 @@
       <c r="K25" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25" t="s">
+        <v>287</v>
+      </c>
+      <c r="M25">
+        <v>4</v>
+      </c>
+      <c r="N25" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="O25" t="s">
+        <v>355</v>
+      </c>
+      <c r="P25" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2543,8 +2878,26 @@
       <c r="J26">
         <v>0.53560224068977191</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K26" t="s">
+        <v>358</v>
+      </c>
+      <c r="L26" t="s">
+        <v>352</v>
+      </c>
+      <c r="M26">
+        <v>4</v>
+      </c>
+      <c r="N26" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="O26" t="s">
+        <v>357</v>
+      </c>
+      <c r="P26" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2575,8 +2928,26 @@
       <c r="J27">
         <v>0.53382453022901966</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K27" t="s">
+        <v>360</v>
+      </c>
+      <c r="L27" t="s">
+        <v>352</v>
+      </c>
+      <c r="M27">
+        <v>5</v>
+      </c>
+      <c r="N27" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="O27" t="s">
+        <v>359</v>
+      </c>
+      <c r="P27" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2607,8 +2978,26 @@
       <c r="J28">
         <v>0.52816260861278796</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K28" t="s">
+        <v>362</v>
+      </c>
+      <c r="L28" t="s">
+        <v>287</v>
+      </c>
+      <c r="M28">
+        <v>4</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="O28" t="s">
+        <v>365</v>
+      </c>
+      <c r="P28" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -2639,8 +3028,26 @@
       <c r="J29">
         <v>0.45548889141916798</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K29" t="s">
+        <v>367</v>
+      </c>
+      <c r="L29" t="s">
+        <v>287</v>
+      </c>
+      <c r="M29">
+        <v>4</v>
+      </c>
+      <c r="N29" t="s">
+        <v>368</v>
+      </c>
+      <c r="O29" t="s">
+        <v>369</v>
+      </c>
+      <c r="P29" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2671,8 +3078,26 @@
       <c r="J30">
         <v>0.45540151986899607</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K30" t="s">
+        <v>370</v>
+      </c>
+      <c r="L30" t="s">
+        <v>371</v>
+      </c>
+      <c r="M30">
+        <v>5</v>
+      </c>
+      <c r="N30" t="s">
+        <v>373</v>
+      </c>
+      <c r="O30" t="s">
+        <v>374</v>
+      </c>
+      <c r="P30" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -2703,8 +3128,26 @@
       <c r="J31">
         <v>0.44465533343947827</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K31" t="s">
+        <v>377</v>
+      </c>
+      <c r="L31" t="s">
+        <v>287</v>
+      </c>
+      <c r="M31">
+        <v>5</v>
+      </c>
+      <c r="N31" s="8">
+        <v>0.13</v>
+      </c>
+      <c r="O31" t="s">
+        <v>375</v>
+      </c>
+      <c r="P31" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -2734,6 +3177,24 @@
       </c>
       <c r="J32">
         <v>0.44270861051173221</v>
+      </c>
+      <c r="K32" t="s">
+        <v>380</v>
+      </c>
+      <c r="L32" t="s">
+        <v>287</v>
+      </c>
+      <c r="M32">
+        <v>6</v>
+      </c>
+      <c r="N32" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="O32" t="s">
+        <v>379</v>
+      </c>
+      <c r="P32" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
completed hand-research of methods
</commit_message>
<xml_diff>
--- a/Midterm Report/Selection of Prompt Engineering Methods/hand-labeled method and implementation considerations.xlsx
+++ b/Midterm Report/Selection of Prompt Engineering Methods/hand-labeled method and implementation considerations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\anlp23-project\Midterm Report\Selection of Prompt Engineering Methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EA03EE-2E6B-4DDC-A420-595989EEC872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C97A2C-3F58-49B4-99B4-DC2869D4DF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="466">
   <si>
     <t>paper title</t>
   </si>
@@ -941,15 +941,6 @@
     <t>Maieutic Prompting</t>
   </si>
   <si>
-    <t>Generated knowledge prompting</t>
-  </si>
-  <si>
-    <t>Active-Prompt</t>
-  </si>
-  <si>
-    <t>Directional-stimulus prompting</t>
-  </si>
-  <si>
     <t>Original GPT-4 Paper</t>
   </si>
   <si>
@@ -1176,15 +1167,280 @@
   </si>
   <si>
     <t>Process Supervision</t>
+  </si>
+  <si>
+    <t>Empirical study of larger LMs capacity to ignore pretraining with new labels</t>
+  </si>
+  <si>
+    <t>ScienceQA</t>
+  </si>
+  <si>
+    <t>Requires fine tuning. Possibly implementable with GPT-4</t>
+  </si>
+  <si>
+    <t>Metaprompt</t>
+  </si>
+  <si>
+    <t>Metaprompting seems to be similar to chain-of-thought prompting and other techniques, loosely defined</t>
+  </si>
+  <si>
+    <t>Role-Playing</t>
+  </si>
+  <si>
+    <t>A feedback loop for agentic behavior would need to be established</t>
+  </si>
+  <si>
+    <t>Wikidata, QUEST, MultiSpanQA</t>
+  </si>
+  <si>
+    <t>20-30%</t>
+  </si>
+  <si>
+    <t>Can be implemented few-shot or zero-shot. There are several variants - Joint, 2-Step, Factored, Factor+Revise, and each has varying numbers of steps</t>
+  </si>
+  <si>
+    <t>Pre-trained Prompt Tuning</t>
+  </si>
+  <si>
+    <t>SST, YahooAns, RACE, BoolQ, RTE, CB</t>
+  </si>
+  <si>
+    <t>GLUE</t>
+  </si>
+  <si>
+    <t>Includes CoT, other prompting strategies</t>
+  </si>
+  <si>
+    <t>Suggests using LM evaluations of responses</t>
+  </si>
+  <si>
+    <t>GSM8K, MultiArith, MathQA, Date Understanding, Penguins</t>
+  </si>
+  <si>
+    <t>5-20%</t>
+  </si>
+  <si>
+    <t>Selecting chains with more reasoning steps via prompting or among outputs improves performance</t>
+  </si>
+  <si>
+    <t>Uses soft prompts and embeddings</t>
+  </si>
+  <si>
+    <t>Unclear</t>
+  </si>
+  <si>
+    <t>Decomposed Prompting</t>
+  </si>
+  <si>
+    <t>Requires a library of LLMs for subtasks</t>
+  </si>
+  <si>
+    <t>GSM-IC</t>
+  </si>
+  <si>
+    <t>Not very generalizable as it uses a specialized dataset. The techniques may be somewhat useful though</t>
+  </si>
+  <si>
+    <t>Various, Instruction to Ignore Irrelevant Information</t>
+  </si>
+  <si>
+    <t>Reasoning via Planning</t>
+  </si>
+  <si>
+    <t>30%+</t>
+  </si>
+  <si>
+    <t>Blocksworld, GSM8K, PrOntoQA</t>
+  </si>
+  <si>
+    <t>Building a world model via prompts. Requires monte carlo tree search, reward functions, access to probabilities</t>
+  </si>
+  <si>
+    <t>EvoPrompt</t>
+  </si>
+  <si>
+    <t>15-25%</t>
+  </si>
+  <si>
+    <t>Plan-and-Solve Prompting</t>
+  </si>
+  <si>
+    <t>Demonstrate-Search-Predict</t>
+  </si>
+  <si>
+    <t>REFINER</t>
+  </si>
+  <si>
+    <t>MultiArith, AddSub, GSM8K, AQUA, SingleEq, SVAMP, CommonSenseQA, StrategyQA, Last Letters, Coin Flip</t>
+  </si>
+  <si>
+    <t>2.5-5%</t>
+  </si>
+  <si>
+    <t>Requires connecting LLMs to evolutionary algoirithms</t>
+  </si>
+  <si>
+    <t>SAMSum, ASSET</t>
+  </si>
+  <si>
+    <t>Discusses prompt injection</t>
+  </si>
+  <si>
+    <t>Autoprompt</t>
+  </si>
+  <si>
+    <t>10-20%</t>
+  </si>
+  <si>
+    <t>Create prompts via a gradient guided search. Focuses on classical NLP tasks. Sadly requires access to probabilities</t>
+  </si>
+  <si>
+    <t>Demonstrates that LLMs can be made to follow moral principles</t>
+  </si>
+  <si>
+    <t>Chaining</t>
+  </si>
+  <si>
+    <t>Peer review writing, flashcards</t>
+  </si>
+  <si>
+    <t>Unique tasks. Transparent and controllable process they implemented via a GUI</t>
+  </si>
+  <si>
+    <t>Prompting for Reliability</t>
+  </si>
+  <si>
+    <t>Methods: Use randomly sampled examples from all domains in few shot, include debiased examples, ask for confidence, include knowledge.</t>
+  </si>
+  <si>
+    <t>40-300% relative gains</t>
+  </si>
+  <si>
+    <t>Pass texts between language model and retrieval model</t>
+  </si>
+  <si>
+    <t>Open-SQuAD, HotPotQA, QReCC</t>
+  </si>
+  <si>
+    <t>For text-to-image</t>
+  </si>
+  <si>
+    <t>Requires hookups to search, code generation, etc. Already done for GPT-4 clearly</t>
+  </si>
+  <si>
+    <t>GSM8K, AQUA-RATE, BigBench, MMLU, SQUAD, TriviaQA, SVAMP, MAWPS</t>
+  </si>
+  <si>
+    <t>3-15%</t>
+  </si>
+  <si>
+    <t>MWP, sNLR, MS</t>
+  </si>
+  <si>
+    <t>Requires training a critic model</t>
+  </si>
+  <si>
+    <t>Ask Me Anything Prompting</t>
+  </si>
+  <si>
+    <t>BoolQ, CB, RTE, ANLI, StoryCloze, AGNews, DBPedia, Amazon, SST, NW, RealTimeQA, WebQs, various others</t>
+  </si>
+  <si>
+    <t>Requires a weak supervision model and a probabilistic graphical model</t>
+  </si>
+  <si>
+    <t>Few-shot Dense Retrieval</t>
+  </si>
+  <si>
+    <t>Fever, SciFact, SciDocs, HotpotQ</t>
+  </si>
+  <si>
+    <t>Using LLMs as query generators for an information retrieval system. Perhaps not technically prompt engineering. Would require a retrieval model to be prompted</t>
+  </si>
+  <si>
+    <t>Com2Sense, CommonSenseQA, CREAK</t>
+  </si>
+  <si>
+    <t>ProntoQA</t>
+  </si>
+  <si>
+    <t>Evaluates chain of thought steps, not labels. Models often fail to plan.</t>
+  </si>
+  <si>
+    <t>Uses weighted MAX-SAT solver to collectiveley infer truth values</t>
+  </si>
+  <si>
+    <t>Requires adding prompter agent, checker module, memory module, ToT controller to an LLM</t>
+  </si>
+  <si>
+    <t>Sudoku</t>
+  </si>
+  <si>
+    <t>10-40%</t>
+  </si>
+  <si>
+    <t>5-15%</t>
+  </si>
+  <si>
+    <t>MC-TACO, QASC, Quoref, WinoGrande, CosmosQA, MultiRC, Essential-Terms</t>
+  </si>
+  <si>
+    <t>Reframing</t>
+  </si>
+  <si>
+    <t>Techniques: pattern reframing, itemizing reframing, decomposition reframing, restraining reframing, specialization reframing. Seems trickly to pick how which methods to implement and how - a lot of interpretration/adaptation would be needed</t>
+  </si>
+  <si>
+    <t>NumerSense, CommonSenseQA, CommonSenseQA2, QASC</t>
+  </si>
+  <si>
+    <t>Generated Knowledge Prompting</t>
+  </si>
+  <si>
+    <t>10-32%</t>
+  </si>
+  <si>
+    <t>Roughly one generated knowledge statement captures most of the gains. Use few shots of knowledge. Could have separate or the same knowledge generating and inference models.</t>
+  </si>
+  <si>
+    <t>Algorithmic Prompting</t>
+  </si>
+  <si>
+    <t>Somewhat limited to algorithmic problems.</t>
+  </si>
+  <si>
+    <t>GSM8K, GSM8K-Hard</t>
+  </si>
+  <si>
+    <t>Chain of Hindsight</t>
+  </si>
+  <si>
+    <t>WebGPT, HH, Summarization</t>
+  </si>
+  <si>
+    <t>Requires sampling from outputs and finetuning. This point is the once-per-week cutoff for citations (0.1428*7 is about one)</t>
+  </si>
+  <si>
+    <t>Optimizing hard (rather than soft vector) prompts with gradient optimization. Mentioned to be cheap on tokens. Prompts can be optimized on small models and transferred to larger models</t>
+  </si>
+  <si>
+    <t>Gradient-Based Prompt Optimization</t>
+  </si>
+  <si>
+    <t>SST, Amazon, AGNEWS</t>
+  </si>
+  <si>
+    <t>0-2%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1255,7 +1511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1275,9 +1531,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1582,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K27" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="K53" workbookViewId="0">
+      <selection activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1631,7 +1888,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>282</v>
@@ -1640,7 +1897,7 @@
         <v>283</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>284</v>
@@ -1696,7 +1953,7 @@
         <v>288</v>
       </c>
       <c r="P2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -1731,22 +1988,22 @@
         <v>6.9009214194273243</v>
       </c>
       <c r="K3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="L3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="O3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="P3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="S3" s="9"/>
     </row>
@@ -1782,22 +2039,22 @@
         <v>5.0354387167528598</v>
       </c>
       <c r="K4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="L4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="O4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="P4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -1844,10 +2101,10 @@
         <v>0.4</v>
       </c>
       <c r="O5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="P5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -1882,22 +2139,22 @@
         <v>2.23906210114813</v>
       </c>
       <c r="K6" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="L6" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M6" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N6" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="O6" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="P6" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -1932,22 +2189,22 @@
         <v>1.9305973178964859</v>
       </c>
       <c r="K7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="L7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="O7" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="P7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -1982,7 +2239,7 @@
         <v>1.7074340242348329</v>
       </c>
       <c r="K8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="L8" t="s">
         <v>287</v>
@@ -1994,10 +2251,10 @@
         <v>0.3</v>
       </c>
       <c r="O8" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="P8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -2041,13 +2298,13 @@
         <v>5</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="O9" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="P9" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -2094,10 +2351,10 @@
         <v>0.7</v>
       </c>
       <c r="O10" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="P10" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -2132,22 +2389,22 @@
         <v>1.252771595523718</v>
       </c>
       <c r="K11" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="L11" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M11" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N11" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="O11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="P11" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -2191,13 +2448,13 @@
         <v>5</v>
       </c>
       <c r="N12" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="O12" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P12" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -2232,22 +2489,22 @@
         <v>1.1179596365535029</v>
       </c>
       <c r="K13" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="L13" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M13" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N13" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="O13" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="P13" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -2282,7 +2539,7 @@
         <v>1.056058333234885</v>
       </c>
       <c r="K14" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>287</v>
@@ -2294,10 +2551,10 @@
         <v>0.11</v>
       </c>
       <c r="O14" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P14" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -2332,22 +2589,22 @@
         <v>0.98534937812037926</v>
       </c>
       <c r="K15" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="L15" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M15" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N15" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="O15" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="P15" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -2394,10 +2651,10 @@
         <v>0.2</v>
       </c>
       <c r="O16" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="P16" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -2441,13 +2698,13 @@
         <v>4</v>
       </c>
       <c r="N17" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="O17" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="P17" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -2482,22 +2739,22 @@
         <v>0.76567923536422988</v>
       </c>
       <c r="K18" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="L18" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="M18">
         <v>5</v>
       </c>
       <c r="N18" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="O18" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="P18" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -2532,22 +2789,22 @@
         <v>0.71290973543928726</v>
       </c>
       <c r="K19" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="L19" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M19" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N19" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="O19" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="P19" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -2591,13 +2848,13 @@
         <v>2</v>
       </c>
       <c r="N20" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="O20" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="P20" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
@@ -2632,22 +2889,22 @@
         <v>0.66922693081589502</v>
       </c>
       <c r="K21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="L21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="O21" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="P21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -2682,22 +2939,22 @@
         <v>0.64824468812237357</v>
       </c>
       <c r="K22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="L22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="O22" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="P22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
@@ -2732,7 +2989,7 @@
         <v>0.63142921575299549</v>
       </c>
       <c r="K23" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="L23" t="s">
         <v>287</v>
@@ -2744,10 +3001,10 @@
         <v>0.4</v>
       </c>
       <c r="O23" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="P23" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
@@ -2782,10 +3039,10 @@
         <v>0.58482189517385985</v>
       </c>
       <c r="K24" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="L24" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="M24">
         <v>4</v>
@@ -2794,7 +3051,7 @@
         <v>0.15</v>
       </c>
       <c r="O24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
@@ -2841,10 +3098,10 @@
         <v>0.1</v>
       </c>
       <c r="O25" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="P25" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
@@ -2879,10 +3136,10 @@
         <v>0.53560224068977191</v>
       </c>
       <c r="K26" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="L26" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="M26">
         <v>4</v>
@@ -2891,10 +3148,10 @@
         <v>0.1</v>
       </c>
       <c r="O26" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="P26" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
@@ -2929,10 +3186,10 @@
         <v>0.53382453022901966</v>
       </c>
       <c r="K27" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="L27" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="M27">
         <v>5</v>
@@ -2941,10 +3198,10 @@
         <v>0.3</v>
       </c>
       <c r="O27" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="P27" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
@@ -2979,7 +3236,7 @@
         <v>0.52816260861278796</v>
       </c>
       <c r="K28" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="L28" t="s">
         <v>287</v>
@@ -2988,13 +3245,13 @@
         <v>4</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="O28" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="P28" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -3029,7 +3286,7 @@
         <v>0.45548889141916798</v>
       </c>
       <c r="K29" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="L29" t="s">
         <v>287</v>
@@ -3038,13 +3295,13 @@
         <v>4</v>
       </c>
       <c r="N29" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="O29" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="P29" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -3079,22 +3336,22 @@
         <v>0.45540151986899607</v>
       </c>
       <c r="K30" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="L30" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="M30">
         <v>5</v>
       </c>
       <c r="N30" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="O30" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="P30" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
@@ -3129,7 +3386,7 @@
         <v>0.44465533343947827</v>
       </c>
       <c r="K31" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="L31" t="s">
         <v>287</v>
@@ -3141,10 +3398,10 @@
         <v>0.13</v>
       </c>
       <c r="O31" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="P31" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
@@ -3179,25 +3436,25 @@
         <v>0.44270861051173221</v>
       </c>
       <c r="K32" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="L32" t="s">
         <v>287</v>
       </c>
       <c r="M32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N32" s="8">
         <v>0.06</v>
       </c>
       <c r="O32" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="P32" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -3228,8 +3485,26 @@
       <c r="J33">
         <v>0.37897826657409323</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K33" t="s">
+        <v>304</v>
+      </c>
+      <c r="L33" t="s">
+        <v>304</v>
+      </c>
+      <c r="M33" t="s">
+        <v>304</v>
+      </c>
+      <c r="N33" t="s">
+        <v>304</v>
+      </c>
+      <c r="O33" t="s">
+        <v>378</v>
+      </c>
+      <c r="P33" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -3263,8 +3538,23 @@
       <c r="K34" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34" t="s">
+        <v>349</v>
+      </c>
+      <c r="M34">
+        <v>4</v>
+      </c>
+      <c r="N34" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="O34" t="s">
+        <v>380</v>
+      </c>
+      <c r="P34" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -3295,8 +3585,23 @@
       <c r="J35">
         <v>0.32361315938304103</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K35" t="s">
+        <v>381</v>
+      </c>
+      <c r="L35" t="s">
+        <v>287</v>
+      </c>
+      <c r="M35" t="s">
+        <v>304</v>
+      </c>
+      <c r="N35" t="s">
+        <v>304</v>
+      </c>
+      <c r="O35" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -3327,8 +3632,23 @@
       <c r="J36">
         <v>0.31133762921471098</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K36" t="s">
+        <v>383</v>
+      </c>
+      <c r="L36" t="s">
+        <v>287</v>
+      </c>
+      <c r="M36">
+        <v>4</v>
+      </c>
+      <c r="N36" t="s">
+        <v>304</v>
+      </c>
+      <c r="O36" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -3362,8 +3682,23 @@
       <c r="K37" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37" t="s">
+        <v>287</v>
+      </c>
+      <c r="M37">
+        <v>3</v>
+      </c>
+      <c r="N37" t="s">
+        <v>386</v>
+      </c>
+      <c r="O37" t="s">
+        <v>387</v>
+      </c>
+      <c r="P37" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -3394,8 +3729,26 @@
       <c r="J38">
         <v>0.30249573901181348</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K38" t="s">
+        <v>388</v>
+      </c>
+      <c r="L38" t="s">
+        <v>287</v>
+      </c>
+      <c r="M38">
+        <v>5</v>
+      </c>
+      <c r="N38" t="s">
+        <v>397</v>
+      </c>
+      <c r="O38" t="s">
+        <v>396</v>
+      </c>
+      <c r="P38" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -3429,8 +3782,23 @@
       <c r="K39" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39" t="s">
+        <v>287</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39" t="s">
+        <v>394</v>
+      </c>
+      <c r="O39" t="s">
+        <v>395</v>
+      </c>
+      <c r="P39" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -3461,8 +3829,26 @@
       <c r="J40">
         <v>0.29727409989322168</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K40" t="s">
+        <v>304</v>
+      </c>
+      <c r="L40" t="s">
+        <v>304</v>
+      </c>
+      <c r="M40" t="s">
+        <v>304</v>
+      </c>
+      <c r="N40" t="s">
+        <v>304</v>
+      </c>
+      <c r="O40" t="s">
+        <v>391</v>
+      </c>
+      <c r="P40" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -3493,8 +3879,26 @@
       <c r="J41">
         <v>0.28286738997947958</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K41" t="s">
+        <v>304</v>
+      </c>
+      <c r="L41" t="s">
+        <v>304</v>
+      </c>
+      <c r="M41" t="s">
+        <v>304</v>
+      </c>
+      <c r="N41" t="s">
+        <v>304</v>
+      </c>
+      <c r="O41" t="s">
+        <v>392</v>
+      </c>
+      <c r="P41" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -3525,8 +3929,23 @@
       <c r="J42">
         <v>0.27184950155199189</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K42" t="s">
+        <v>398</v>
+      </c>
+      <c r="L42" t="s">
+        <v>287</v>
+      </c>
+      <c r="M42">
+        <v>4</v>
+      </c>
+      <c r="N42" t="s">
+        <v>361</v>
+      </c>
+      <c r="O42" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -3557,8 +3976,23 @@
       <c r="J43">
         <v>0.27128301443900782</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K43" t="s">
+        <v>409</v>
+      </c>
+      <c r="L43" t="s">
+        <v>287</v>
+      </c>
+      <c r="M43">
+        <v>2</v>
+      </c>
+      <c r="N43" t="s">
+        <v>413</v>
+      </c>
+      <c r="O43" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -3589,8 +4023,26 @@
       <c r="J44">
         <v>0.26458564726002243</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K44" t="s">
+        <v>402</v>
+      </c>
+      <c r="L44" t="s">
+        <v>349</v>
+      </c>
+      <c r="M44">
+        <v>2</v>
+      </c>
+      <c r="N44" t="s">
+        <v>397</v>
+      </c>
+      <c r="O44" t="s">
+        <v>401</v>
+      </c>
+      <c r="P44" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -3621,8 +4073,26 @@
       <c r="J45">
         <v>0.22432676595922049</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K45" t="s">
+        <v>403</v>
+      </c>
+      <c r="L45" t="s">
+        <v>287</v>
+      </c>
+      <c r="M45">
+        <v>5</v>
+      </c>
+      <c r="N45" t="s">
+        <v>404</v>
+      </c>
+      <c r="O45" t="s">
+        <v>406</v>
+      </c>
+      <c r="P45" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -3653,8 +4123,26 @@
       <c r="J46">
         <v>0.21296637596359169</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K46" t="s">
+        <v>407</v>
+      </c>
+      <c r="L46" t="s">
+        <v>287</v>
+      </c>
+      <c r="M46">
+        <v>4</v>
+      </c>
+      <c r="N46" t="s">
+        <v>408</v>
+      </c>
+      <c r="O46" t="s">
+        <v>414</v>
+      </c>
+      <c r="P46" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -3685,8 +4173,26 @@
       <c r="J47">
         <v>0.20025643698396339</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K47" t="s">
+        <v>304</v>
+      </c>
+      <c r="L47" t="s">
+        <v>304</v>
+      </c>
+      <c r="M47" t="s">
+        <v>304</v>
+      </c>
+      <c r="N47" t="s">
+        <v>304</v>
+      </c>
+      <c r="O47" t="s">
+        <v>416</v>
+      </c>
+      <c r="P47" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -3717,8 +4223,26 @@
       <c r="J48">
         <v>0.19934507969108409</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K48" t="s">
+        <v>417</v>
+      </c>
+      <c r="L48" t="s">
+        <v>287</v>
+      </c>
+      <c r="M48">
+        <v>5</v>
+      </c>
+      <c r="N48" t="s">
+        <v>418</v>
+      </c>
+      <c r="O48" t="s">
+        <v>419</v>
+      </c>
+      <c r="P48" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -3749,8 +4273,26 @@
       <c r="J49">
         <v>0.19634193704577491</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K49" t="s">
+        <v>304</v>
+      </c>
+      <c r="L49" t="s">
+        <v>304</v>
+      </c>
+      <c r="M49" t="s">
+        <v>304</v>
+      </c>
+      <c r="N49" t="s">
+        <v>304</v>
+      </c>
+      <c r="O49" t="s">
+        <v>420</v>
+      </c>
+      <c r="P49" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -3781,8 +4323,26 @@
       <c r="J50">
         <v>0.19503994311521911</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K50" t="s">
+        <v>421</v>
+      </c>
+      <c r="L50" t="s">
+        <v>368</v>
+      </c>
+      <c r="M50">
+        <v>4</v>
+      </c>
+      <c r="N50" t="s">
+        <v>304</v>
+      </c>
+      <c r="O50" t="s">
+        <v>423</v>
+      </c>
+      <c r="P50" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>90</v>
       </c>
@@ -3813,8 +4373,23 @@
       <c r="J51">
         <v>0.1942980981277477</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K51" t="s">
+        <v>424</v>
+      </c>
+      <c r="L51" t="s">
+        <v>287</v>
+      </c>
+      <c r="M51">
+        <v>4</v>
+      </c>
+      <c r="N51" t="s">
+        <v>304</v>
+      </c>
+      <c r="O51" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>92</v>
       </c>
@@ -3845,8 +4420,26 @@
       <c r="J52">
         <v>0.19091344742643501</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K52" t="s">
+        <v>410</v>
+      </c>
+      <c r="L52" t="s">
+        <v>287</v>
+      </c>
+      <c r="M52">
+        <v>4</v>
+      </c>
+      <c r="N52" t="s">
+        <v>426</v>
+      </c>
+      <c r="O52" t="s">
+        <v>427</v>
+      </c>
+      <c r="P52" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>94</v>
       </c>
@@ -3877,8 +4470,26 @@
       <c r="J53">
         <v>0.18476000216517699</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K53" t="s">
+        <v>304</v>
+      </c>
+      <c r="L53" t="s">
+        <v>304</v>
+      </c>
+      <c r="M53" t="s">
+        <v>304</v>
+      </c>
+      <c r="N53" t="s">
+        <v>304</v>
+      </c>
+      <c r="O53" t="s">
+        <v>429</v>
+      </c>
+      <c r="P53" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>96</v>
       </c>
@@ -3912,8 +4523,23 @@
       <c r="K54" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L54" t="s">
+        <v>287</v>
+      </c>
+      <c r="M54">
+        <v>4</v>
+      </c>
+      <c r="N54" t="s">
+        <v>365</v>
+      </c>
+      <c r="O54" t="s">
+        <v>430</v>
+      </c>
+      <c r="P54" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>98</v>
       </c>
@@ -3944,8 +4570,26 @@
       <c r="J55">
         <v>0.17364158850799219</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K55" t="s">
+        <v>411</v>
+      </c>
+      <c r="L55" t="s">
+        <v>287</v>
+      </c>
+      <c r="M55">
+        <v>5</v>
+      </c>
+      <c r="N55" t="s">
+        <v>432</v>
+      </c>
+      <c r="O55" t="s">
+        <v>434</v>
+      </c>
+      <c r="P55" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>99</v>
       </c>
@@ -3976,8 +4620,26 @@
       <c r="J56">
         <v>0.16990593846999499</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K56" t="s">
+        <v>435</v>
+      </c>
+      <c r="L56" t="s">
+        <v>287</v>
+      </c>
+      <c r="M56">
+        <v>5</v>
+      </c>
+      <c r="N56" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="O56" t="s">
+        <v>437</v>
+      </c>
+      <c r="P56" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>100</v>
       </c>
@@ -4008,8 +4670,26 @@
       <c r="J57">
         <v>0.1672729824948033</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K57" t="s">
+        <v>438</v>
+      </c>
+      <c r="L57" t="s">
+        <v>349</v>
+      </c>
+      <c r="M57">
+        <v>4</v>
+      </c>
+      <c r="N57" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="O57" t="s">
+        <v>440</v>
+      </c>
+      <c r="P57" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>102</v>
       </c>
@@ -4043,8 +4723,23 @@
       <c r="K58" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L58" t="s">
+        <v>287</v>
+      </c>
+      <c r="M58">
+        <v>4</v>
+      </c>
+      <c r="N58" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="O58" t="s">
+        <v>444</v>
+      </c>
+      <c r="P58" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>103</v>
       </c>
@@ -4075,8 +4770,26 @@
       <c r="J59">
         <v>0.16192857897081411</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K59" t="s">
+        <v>291</v>
+      </c>
+      <c r="L59" t="s">
+        <v>287</v>
+      </c>
+      <c r="M59">
+        <v>5</v>
+      </c>
+      <c r="N59" t="s">
+        <v>447</v>
+      </c>
+      <c r="O59" t="s">
+        <v>445</v>
+      </c>
+      <c r="P59" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>105</v>
       </c>
@@ -4107,8 +4820,26 @@
       <c r="J60">
         <v>0.1578470980446437</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K60" t="s">
+        <v>450</v>
+      </c>
+      <c r="L60" t="s">
+        <v>287</v>
+      </c>
+      <c r="M60">
+        <v>4</v>
+      </c>
+      <c r="N60" t="s">
+        <v>448</v>
+      </c>
+      <c r="O60" t="s">
+        <v>451</v>
+      </c>
+      <c r="P60" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>107</v>
       </c>
@@ -4140,10 +4871,25 @@
         <v>0.15456272931786141</v>
       </c>
       <c r="K61" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+        <v>453</v>
+      </c>
+      <c r="L61" t="s">
+        <v>368</v>
+      </c>
+      <c r="M61">
+        <v>3</v>
+      </c>
+      <c r="N61" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="O61" t="s">
+        <v>455</v>
+      </c>
+      <c r="P61" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>108</v>
       </c>
@@ -4174,8 +4920,26 @@
       <c r="J62">
         <v>0.15224059419486069</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K62" t="s">
+        <v>456</v>
+      </c>
+      <c r="L62" t="s">
+        <v>368</v>
+      </c>
+      <c r="M62">
+        <v>4</v>
+      </c>
+      <c r="N62" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="O62" t="s">
+        <v>457</v>
+      </c>
+      <c r="P62" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>110</v>
       </c>
@@ -4206,8 +4970,26 @@
       <c r="J63">
         <v>0.15081990823327751</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K63" t="s">
+        <v>304</v>
+      </c>
+      <c r="L63" t="s">
+        <v>304</v>
+      </c>
+      <c r="M63" t="s">
+        <v>304</v>
+      </c>
+      <c r="N63" t="s">
+        <v>304</v>
+      </c>
+      <c r="O63" t="s">
+        <v>443</v>
+      </c>
+      <c r="P63" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>112</v>
       </c>
@@ -4238,8 +5020,26 @@
       <c r="J64">
         <v>0.14753579386393459</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K64" t="s">
+        <v>463</v>
+      </c>
+      <c r="L64" t="s">
+        <v>287</v>
+      </c>
+      <c r="M64">
+        <v>4</v>
+      </c>
+      <c r="N64" t="s">
+        <v>465</v>
+      </c>
+      <c r="O64" t="s">
+        <v>462</v>
+      </c>
+      <c r="P64" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>114</v>
       </c>
@@ -4270,8 +5070,23 @@
       <c r="J65">
         <v>0.143097693189494</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K65" t="s">
+        <v>459</v>
+      </c>
+      <c r="M65">
+        <v>5</v>
+      </c>
+      <c r="N65" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="O65" t="s">
+        <v>461</v>
+      </c>
+      <c r="P65" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>115</v>
       </c>
@@ -4302,11 +5117,8 @@
       <c r="J66">
         <v>0.1407490908707828</v>
       </c>
-      <c r="K66" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>117</v>
       </c>
@@ -4338,7 +5150,7 @@
         <v>0.1325258059403561</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>118</v>
       </c>
@@ -4370,7 +5182,7 @@
         <v>0.13125230137418131</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>120</v>
       </c>
@@ -4402,7 +5214,7 @@
         <v>0.1284441136443728</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>123</v>
       </c>
@@ -4434,7 +5246,7 @@
         <v>0.12556322350312701</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>124</v>
       </c>
@@ -4466,7 +5278,7 @@
         <v>0.1190740187342867</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>126</v>
       </c>
@@ -4498,7 +5310,7 @@
         <v>0.1121633829796103</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>128</v>
       </c>
@@ -4530,7 +5342,7 @@
         <v>0.1018828738867036</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>130</v>
       </c>
@@ -4562,7 +5374,7 @@
         <v>9.864753644344397E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>132</v>
       </c>
@@ -4594,7 +5406,7 @@
         <v>9.6968749784157426E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>134</v>
       </c>
@@ -4626,7 +5438,7 @@
         <v>9.6463538390330283E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>136</v>
       </c>
@@ -4658,7 +5470,7 @@
         <v>9.46504304825702E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>138</v>
       </c>
@@ -4690,7 +5502,7 @@
         <v>9.1209934876282261E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>140</v>
       </c>
@@ -4722,7 +5534,7 @@
         <v>9.1166835316776149E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>141</v>
       </c>
@@ -5266,7 +6078,7 @@
         <v>5.7869797902564767E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>170</v>
       </c>
@@ -5298,7 +6110,7 @@
         <v>5.7760321334283563E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>172</v>
       </c>
@@ -5330,7 +6142,7 @@
         <v>5.7453730502123913E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>174</v>
       </c>
@@ -5362,7 +6174,7 @@
         <v>5.2436798536494633E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>176</v>
       </c>
@@ -5394,7 +6206,7 @@
         <v>5.2046147587294547E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>178</v>
       </c>
@@ -5426,7 +6238,7 @@
         <v>5.1506659850452399E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>181</v>
       </c>
@@ -5458,7 +6270,7 @@
         <v>5.0726098580666047E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>183</v>
       </c>
@@ -5490,7 +6302,7 @@
         <v>4.9304054327021257E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>185</v>
       </c>
@@ -5522,7 +6334,7 @@
         <v>4.7680831849081291E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>187</v>
       </c>
@@ -5554,7 +6366,7 @@
         <v>4.4878655035075259E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>189</v>
       </c>
@@ -5585,11 +6397,8 @@
       <c r="J106">
         <v>4.1226128488322772E-2</v>
       </c>
-      <c r="K106" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>190</v>
       </c>
@@ -5621,7 +6430,7 @@
         <v>4.0289152148574113E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>192</v>
       </c>
@@ -5653,7 +6462,7 @@
         <v>3.8322835500137008E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>194</v>
       </c>
@@ -5685,7 +6494,7 @@
         <v>3.615791552578114E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>196</v>
       </c>
@@ -5717,7 +6526,7 @@
         <v>3.6106848499292743E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>198</v>
       </c>
@@ -5749,7 +6558,7 @@
         <v>3.4972246386761691E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>200</v>
       </c>

</xml_diff>